<commit_message>
some minor changes for testing purposes
</commit_message>
<xml_diff>
--- a/tests/accounts.xlsx
+++ b/tests/accounts.xlsx
@@ -1,26 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rango/Desktop/Rango/Projects/SoftAI/facebook-scraper/tests/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09BC9C68-EA2C-E04E-98F8-E7342FA56700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10814"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499B2BD1-BAC2-524F-B93D-B1F57B3E5FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+  <si>
+    <t>abendukidze</t>
+  </si>
+  <si>
+    <t>lbokeria</t>
+  </si>
+  <si>
+    <t>vakho.kaloiani</t>
+  </si>
   <si>
     <t>niazi.chitidze</t>
   </si>
@@ -52,9 +68,6 @@
     <t>giorgi.noniashvili.7</t>
   </si>
   <si>
-    <t>giorgi.turkiashvili</t>
-  </si>
-  <si>
     <t>nanuka.mikeladze</t>
   </si>
   <si>
@@ -67,19 +80,256 @@
     <t>malkhaz.pataraia</t>
   </si>
   <si>
+    <t>vaska.matitaishvili</t>
+  </si>
+  <si>
+    <t>tkutaladze</t>
+  </si>
+  <si>
+    <t>nuka.zurashvili</t>
+  </si>
+  <si>
+    <t>abashidzeanano</t>
+  </si>
+  <si>
+    <t>rgvasalia</t>
+  </si>
+  <si>
+    <t>kato.kopaleishvili</t>
+  </si>
+  <si>
+    <t>ejanelidze</t>
+  </si>
+  <si>
+    <t>gkandelaki</t>
+  </si>
+  <si>
+    <t>gvantsakvara</t>
+  </si>
+  <si>
+    <t>ilia.rurua</t>
+  </si>
+  <si>
+    <t>v.khorava</t>
+  </si>
+  <si>
+    <t>fsixf6</t>
+  </si>
+  <si>
+    <t>tornike.toko.9</t>
+  </si>
+  <si>
+    <t>iviko.shengelia</t>
+  </si>
+  <si>
+    <t>lile.chxetiani</t>
+  </si>
+  <si>
+    <t>giga.bedineishvili</t>
+  </si>
+  <si>
+    <t>natia.samushia</t>
+  </si>
+  <si>
+    <t>levanrami</t>
+  </si>
+  <si>
+    <t>Georgi.Tabagari</t>
+  </si>
+  <si>
+    <t>giorgi.pachuashvili.90</t>
+  </si>
+  <si>
+    <t>gchitidze</t>
+  </si>
+  <si>
+    <t>giorgi.cinaridze.1</t>
+  </si>
+  <si>
+    <t>irena.sturua</t>
+  </si>
+  <si>
+    <t>zurab.chilingarashvili</t>
+  </si>
+  <si>
+    <t>BRUTYAN.EDG</t>
+  </si>
+  <si>
+    <t>jabuamaka</t>
+  </si>
+  <si>
+    <t>DimaChikvaidze</t>
+  </si>
+  <si>
+    <t>nino.ordenidze</t>
+  </si>
+  <si>
+    <t>magda.bobokhidze</t>
+  </si>
+  <si>
+    <t>ani.qartlelishvili</t>
+  </si>
+  <si>
+    <t>lukakato1977</t>
+  </si>
+  <si>
+    <t>mari.akhsiashvili</t>
+  </si>
+  <si>
+    <t>tiniko.goguadze</t>
+  </si>
+  <si>
+    <t>amiran.dzotsenidze</t>
+  </si>
+  <si>
+    <t>lasha.migineishvili1</t>
+  </si>
+  <si>
+    <t>irakli.bobokhidze.9</t>
+  </si>
+  <si>
+    <t>david.paitchadze</t>
+  </si>
+  <si>
+    <t>shota.berulava.5</t>
+  </si>
+  <si>
+    <t>mariam.khokhobaia</t>
+  </si>
+  <si>
+    <t>beqa.papashvili.1</t>
+  </si>
+  <si>
+    <t>fruii</t>
+  </si>
+  <si>
+    <t>tsisiakir</t>
+  </si>
+  <si>
+    <t>giorgi.taba</t>
+  </si>
+  <si>
+    <t>S.Balanchine</t>
+  </si>
+  <si>
+    <t>d.targamadze</t>
+  </si>
+  <si>
+    <t>mariam.mindiashvili.7</t>
+  </si>
+  <si>
+    <t>nana.goderdzishvili.56</t>
+  </si>
+  <si>
+    <t>alexander.tsnobiladze.7</t>
+  </si>
+  <si>
+    <t>nana.chartolani</t>
+  </si>
+  <si>
+    <t>irakli.khvadagiani.7</t>
+  </si>
+  <si>
+    <t>anoania</t>
+  </si>
+  <si>
+    <t>FokiPachulia</t>
+  </si>
+  <si>
+    <t>spalavandishvili</t>
+  </si>
+  <si>
+    <t>avtandil.guruli</t>
+  </si>
+  <si>
+    <t>zurab.janiashvili.3</t>
+  </si>
+  <si>
+    <t>Marikuna28</t>
+  </si>
+  <si>
+    <t>tea.kotua.5</t>
+  </si>
+  <si>
+    <t>gvancakika</t>
+  </si>
+  <si>
+    <t>sopho.dvali.7</t>
+  </si>
+  <si>
+    <t>rati.tsiklauri</t>
+  </si>
+  <si>
+    <t>giomeladze</t>
+  </si>
+  <si>
+    <t>teko.dzidziguri</t>
+  </si>
+  <si>
+    <t>rusudan.chergoleishvili</t>
+  </si>
+  <si>
+    <t>khalibegmagamedovi</t>
+  </si>
+  <si>
+    <t>iamnikazurashvili</t>
+  </si>
+  <si>
+    <t>tamar.samkharadze.737</t>
+  </si>
+  <si>
+    <t>dalitabagua</t>
+  </si>
+  <si>
+    <t>irakli.areshidze</t>
+  </si>
+  <si>
+    <t>shota.mindeli</t>
+  </si>
+  <si>
+    <t>ninuca.chergoleishvili</t>
+  </si>
+  <si>
+    <t>grizelda.Tsereteli</t>
+  </si>
+  <si>
+    <t>natia.kordzadze.7</t>
+  </si>
+  <si>
+    <t>tamta.otiashvili</t>
+  </si>
+  <si>
+    <t>medeaivan</t>
+  </si>
+  <si>
+    <t>katherine.earnshaw.942</t>
+  </si>
+  <si>
+    <t>tea.gurabanidze</t>
+  </si>
+  <si>
+    <t>sandro.levanishvili</t>
+  </si>
+  <si>
+    <t>chikkovani</t>
+  </si>
+  <si>
+    <t>ani.kakhidze.7</t>
+  </si>
+  <si>
+    <t>georgetserodze</t>
+  </si>
+  <si>
+    <t>Trockigio</t>
+  </si>
+  <si>
     <t>100000105738767</t>
   </si>
   <si>
-    <t>vaska.matitaishvili</t>
-  </si>
-  <si>
-    <t>tkutaladze</t>
-  </si>
-  <si>
-    <t>vakho.kaloiani</t>
-  </si>
-  <si>
-    <t>abendukidze</t>
+    <t>100009508128159</t>
+  </si>
+  <si>
+    <t>100006589183993</t>
   </si>
 </sst>
 </file>
@@ -456,27 +706,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A97"/>
+  <dimension ref="A1:A101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
@@ -540,7 +793,7 @@
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1" t="s">
+      <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
@@ -550,28 +803,424 @@
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>17</v>
+      <c r="A18" s="1" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>1</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="1"/>
+      <c r="A83" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" s="1"/>
+      <c r="A86" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A97" s="1"/>
+      <c r="A97" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>97</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>